<commit_message>
ccbottlersus-sand update Hunter's changes
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/REDSCORE/Data/KPITemplateV4.6.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/REDSCORE/Data/KPITemplateV4.6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,6 +21,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$Q$70</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$I$63</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Survey!$A$1:$E$28</definedName>
   </definedNames>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="284">
   <si>
     <t xml:space="preserve">Region</t>
   </si>
@@ -1215,29 +1216,29 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.3886639676113"/>
@@ -1330,7 +1331,7 @@
       </c>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" s="5" customFormat="true" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1343,16 +1344,18 @@
       <c r="D3" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="0"/>
+      <c r="J3" s="5"/>
       <c r="L3" s="4" t="s">
         <v>23</v>
       </c>
@@ -1362,7 +1365,7 @@
       </c>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" s="5" customFormat="true" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1384,7 +1387,9 @@
       <c r="I4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="0"/>
+      <c r="K4" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="L4" s="4" t="s">
         <v>23</v>
       </c>
@@ -3558,13 +3563,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.89068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
@@ -4636,15 +4641,15 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.67611336032389"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
@@ -5314,11 +5319,11 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.2388663967611"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.5627530364373"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
@@ -5517,10 +5522,10 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5977,18 +5982,18 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.5951417004049"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.6315789473684"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.0607287449393"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6217,7 +6222,7 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>